<commit_message>
brought back indep isotherm reg feature
</commit_message>
<xml_diff>
--- a/case2_Glu-Fru/glu_fru_launch.xlsx
+++ b/case2_Glu-Fru/glu_fru_launch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case2_Glu-Fru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62956081-1770-4BB5-9272-340D4C58AE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BE5D06-6486-40F0-ACF6-6AFD0363E476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glucose" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -520,12 +520,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2216,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2322,7 +2317,7 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="29">
         <f t="shared" ref="C2:C27" si="0">B2*$K$5</f>
         <v>0</v>
       </c>
@@ -2336,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="19">
-        <f t="shared" ref="G2:G33" si="1">E3*0.000001</f>
+        <f t="shared" ref="G2:G28" si="1">E3*0.000001</f>
         <v>0</v>
       </c>
       <c r="H2" s="19">
@@ -2399,7 +2394,7 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="29">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
@@ -2417,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="19">
-        <f t="shared" ref="H3:H33" si="2">F3*0.000001</f>
+        <f t="shared" ref="H3:H28" si="2">F3*0.000001</f>
         <v>0</v>
       </c>
       <c r="M3" s="3"/>
@@ -2433,7 +2428,7 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="29">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
@@ -2471,7 +2466,7 @@
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
@@ -2510,7 +2505,7 @@
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="29">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
@@ -2539,7 +2534,7 @@
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="29">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2568,7 +2563,7 @@
       <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="29">
         <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
@@ -2598,7 +2593,7 @@
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="29">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
@@ -2628,7 +2623,7 @@
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="29">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
@@ -2658,7 +2653,7 @@
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
@@ -2687,7 +2682,7 @@
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2717,7 +2712,7 @@
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <f t="shared" si="0"/>
         <v>6.6</v>
       </c>
@@ -2747,7 +2742,7 @@
       <c r="B14" s="1">
         <v>12</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="29">
         <f t="shared" si="0"/>
         <v>7.1999999999999993</v>
       </c>
@@ -2777,7 +2772,7 @@
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="29">
         <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
@@ -2807,7 +2802,7 @@
       <c r="B16" s="1">
         <v>14</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="29">
         <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
@@ -2837,7 +2832,7 @@
       <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2867,7 +2862,7 @@
       <c r="B18" s="1">
         <v>16</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="29">
         <f t="shared" si="0"/>
         <v>9.6</v>
       </c>
@@ -2897,7 +2892,7 @@
       <c r="B19" s="1">
         <v>17</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="29">
         <f t="shared" si="0"/>
         <v>10.199999999999999</v>
       </c>
@@ -2927,7 +2922,7 @@
       <c r="B20" s="1">
         <v>18</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="29">
         <f t="shared" si="0"/>
         <v>10.799999999999999</v>
       </c>
@@ -2957,7 +2952,7 @@
       <c r="B21" s="1">
         <v>19</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="29">
         <f t="shared" si="0"/>
         <v>11.4</v>
       </c>
@@ -2987,7 +2982,7 @@
       <c r="B22" s="1">
         <v>20</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="29">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -3017,7 +3012,7 @@
       <c r="B23" s="1">
         <v>21</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="29">
         <f t="shared" si="0"/>
         <v>12.6</v>
       </c>
@@ -3047,7 +3042,7 @@
       <c r="B24" s="1">
         <v>22</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="29">
         <f t="shared" si="0"/>
         <v>13.2</v>
       </c>
@@ -3077,7 +3072,7 @@
       <c r="B25" s="1">
         <v>23</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="29">
         <f t="shared" si="0"/>
         <v>13.799999999999999</v>
       </c>
@@ -3107,7 +3102,7 @@
       <c r="B26" s="1">
         <v>24</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="29">
         <f t="shared" si="0"/>
         <v>14.399999999999999</v>
       </c>
@@ -3137,7 +3132,7 @@
       <c r="B27" s="1">
         <v>25</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -3167,8 +3162,8 @@
       <c r="B28" s="24">
         <v>26</v>
       </c>
-      <c r="C28" s="33">
-        <f t="shared" ref="C28:C33" si="3">B28*$K$5</f>
+      <c r="C28" s="30">
+        <f t="shared" ref="C28" si="3">B28*$K$5</f>
         <v>15.6</v>
       </c>
       <c r="D28" s="25">
@@ -3190,154 +3185,142 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -3539,7 +3522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69A9A7F-E02F-49C0-A7A6-C1ECC304481E}">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
@@ -3785,22 +3768,22 @@
       <c r="E18" s="13">
         <v>117.21</v>
       </c>
-      <c r="J18" s="34" t="s">
+      <c r="J18" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="O18" s="34" t="s">
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
+      <c r="O18" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="36"/>
-      <c r="S18" s="34" t="s">
+      <c r="P18" s="32"/>
+      <c r="Q18" s="33"/>
+      <c r="S18" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="33"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
@@ -4112,15 +4095,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048117A934AEAC441AF47E945F1AED0C0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7272456f5b53c8ae1c345851aef95d27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c39f1452-4462-4979-941b-c1317cfd14ce" xmlns:ns3="60199b31-2299-4531-8872-a3eaba744cbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16ed4d68a838bfbb08a7468a1792fb8f" ns2:_="" ns3:_="">
     <xsd:import namespace="c39f1452-4462-4979-941b-c1317cfd14ce"/>
@@ -4377,15 +4351,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF42137A-B7F2-4A60-BAD9-4B8683F12BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4402,4 +4377,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>